<commit_message>
Upload and insert worksgit add .git add .
</commit_message>
<xml_diff>
--- a/public/exports/cases mock data insert.xlsx
+++ b/public/exports/cases mock data insert.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darryllrobinson/Documents/projects/collections/public/exports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB235B85-7617-D044-BB4D-5A617B28458F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5B2375-52DE-E34F-BAEE-D5F4353FA7EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16000"/>
+    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="accounts" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="32">
   <si>
     <t>id</t>
   </si>
@@ -121,9 +121,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -610,7 +610,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -965,10 +965,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1070,8 +1072,8 @@
       <c r="K2" t="s">
         <v>17</v>
       </c>
-      <c r="L2" t="s">
-        <v>17</v>
+      <c r="L2" s="1">
+        <v>43944.5</v>
       </c>
       <c r="M2" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Upload and insert per table - need to DRY the code still
</commit_message>
<xml_diff>
--- a/public/exports/cases mock data insert.xlsx
+++ b/public/exports/cases mock data insert.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darryllrobinson/Documents/projects/collections/public/exports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5B2375-52DE-E34F-BAEE-D5F4353FA7EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74427B60-3378-4D47-8197-55A7E423C8CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="32">
-  <si>
-    <t>id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="31">
   <si>
     <t>AccountNumber</t>
   </si>
@@ -966,32 +963,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1034,46 +1028,43 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="B2" s="1">
         <v>43944.5</v>
       </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="1">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1">
         <v>43944.5</v>
       </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
       <c r="H2" t="s">
         <v>16</v>
       </c>
       <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="1">
+        <v>43944.5</v>
+      </c>
+      <c r="L2" t="s">
         <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="1">
-        <v>43944.5</v>
       </c>
       <c r="M2" t="s">
         <v>18</v>
@@ -1081,43 +1072,40 @@
       <c r="N2" t="s">
         <v>19</v>
       </c>
-      <c r="O2" t="s">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="B3" s="1">
         <v>43945.5</v>
       </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1">
         <v>43945.5</v>
       </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
       <c r="H3" t="s">
         <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L3" t="s">
         <v>17</v>
@@ -1128,43 +1116,40 @@
       <c r="N3" t="s">
         <v>19</v>
       </c>
-      <c r="O3" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="1">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1">
         <v>43946.5</v>
       </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="1">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1">
         <v>43946.5</v>
       </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
       <c r="H4" t="s">
         <v>16</v>
       </c>
       <c r="I4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L4" t="s">
         <v>17</v>
@@ -1175,43 +1160,40 @@
       <c r="N4" t="s">
         <v>19</v>
       </c>
-      <c r="O4" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="1">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1">
         <v>43947.5</v>
       </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="1">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1">
         <v>43947.5</v>
       </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
       <c r="H5" t="s">
         <v>16</v>
       </c>
       <c r="I5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L5" t="s">
         <v>17</v>
@@ -1222,43 +1204,40 @@
       <c r="N5" t="s">
         <v>19</v>
       </c>
-      <c r="O5" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="1">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1">
         <v>43948.5</v>
       </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="1">
+        <v>15</v>
+      </c>
+      <c r="F6" s="1">
         <v>43948.5</v>
       </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
       <c r="H6" t="s">
         <v>16</v>
       </c>
       <c r="I6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L6" t="s">
         <v>17</v>
@@ -1269,43 +1248,40 @@
       <c r="N6" t="s">
         <v>19</v>
       </c>
-      <c r="O6" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="1">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="1">
         <v>43949.5</v>
       </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="1">
+        <v>15</v>
+      </c>
+      <c r="F7" s="1">
         <v>43949.5</v>
       </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
       <c r="H7" t="s">
         <v>16</v>
       </c>
       <c r="I7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L7" t="s">
         <v>17</v>
@@ -1316,43 +1292,40 @@
       <c r="N7" t="s">
         <v>19</v>
       </c>
-      <c r="O7" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="1">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1">
         <v>43950.5</v>
       </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="1">
+        <v>15</v>
+      </c>
+      <c r="F8" s="1">
         <v>43950.5</v>
       </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
       <c r="H8" t="s">
         <v>16</v>
       </c>
       <c r="I8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L8" t="s">
         <v>17</v>
@@ -1363,43 +1336,40 @@
       <c r="N8" t="s">
         <v>19</v>
       </c>
-      <c r="O8" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="1">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1">
         <v>43951.5</v>
       </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="1">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1">
         <v>43951.5</v>
       </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
       <c r="H9" t="s">
         <v>16</v>
       </c>
       <c r="I9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L9" t="s">
         <v>17</v>
@@ -1410,43 +1380,40 @@
       <c r="N9" t="s">
         <v>19</v>
       </c>
-      <c r="O9" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="1">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1">
         <v>43952.5</v>
       </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="1">
+        <v>15</v>
+      </c>
+      <c r="F10" s="1">
         <v>43952.5</v>
       </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
       <c r="H10" t="s">
         <v>16</v>
       </c>
       <c r="I10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L10" t="s">
         <v>17</v>
@@ -1457,43 +1424,40 @@
       <c r="N10" t="s">
         <v>19</v>
       </c>
-      <c r="O10" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="1">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1">
         <v>43953.5</v>
       </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="1">
+        <v>15</v>
+      </c>
+      <c r="F11" s="1">
         <v>43953.5</v>
       </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
       <c r="H11" t="s">
         <v>16</v>
       </c>
       <c r="I11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L11" t="s">
         <v>17</v>
@@ -1504,43 +1468,40 @@
       <c r="N11" t="s">
         <v>19</v>
       </c>
-      <c r="O11" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="1">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1">
         <v>43954.5</v>
       </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="1">
+        <v>15</v>
+      </c>
+      <c r="F12" s="1">
         <v>43954.5</v>
       </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
       <c r="H12" t="s">
         <v>16</v>
       </c>
       <c r="I12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L12" t="s">
         <v>17</v>
@@ -1551,43 +1512,40 @@
       <c r="N12" t="s">
         <v>19</v>
       </c>
-      <c r="O12" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="1">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="1">
         <v>43955.5</v>
       </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="1">
+        <v>15</v>
+      </c>
+      <c r="F13" s="1">
         <v>43955.5</v>
       </c>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
       <c r="H13" t="s">
         <v>16</v>
       </c>
       <c r="I13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L13" t="s">
         <v>17</v>
@@ -1597,9 +1555,6 @@
       </c>
       <c r="N13" t="s">
         <v>19</v>
-      </c>
-      <c r="O13" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>